<commit_message>
-Update base class and code correction
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PathmazingPC\Stars\appiumtest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35686CE4-CC1E-40B1-8A14-4140D09CC47F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D849205A-6436-4E74-967D-D922F771EEA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
   <si>
     <t>User Name</t>
   </si>
@@ -81,9 +81,6 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>Mobile number</t>
-  </si>
-  <si>
     <t>Nationality</t>
   </si>
   <si>
@@ -103,6 +100,36 @@
   </si>
   <si>
     <t>Lastest Reward Reason</t>
+  </si>
+  <si>
+    <t>QA Tester</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>01/08/2017</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>Phnom Penh</t>
+  </si>
+  <si>
+    <t>Thank for your hard working on the stars app feature, especially try to finish all task on time.</t>
+  </si>
+  <si>
+    <t>Monnyka Pin</t>
+  </si>
+  <si>
+    <t>Time Off Reason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I have to go to the bank tomorrow </t>
   </si>
 </sst>
 </file>
@@ -184,18 +211,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -477,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF5"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,32 +525,32 @@
     <col min="8" max="8" width="11.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" style="1" customWidth="1"/>
     <col min="10" max="11" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="14.140625" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
-    <col min="16" max="16" width="13" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" customWidth="1"/>
-    <col min="19" max="19" width="23.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" customWidth="1"/>
+    <col min="15" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="23.140625" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B2"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
@@ -554,70 +584,68 @@
       <c r="AC3" s="4"/>
       <c r="AD3" s="4"/>
       <c r="AE3" s="4"/>
-      <c r="AF3" s="4"/>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="K4" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="R4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="S4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
+      <c r="S4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="T4" s="6"/>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
@@ -644,6 +672,34 @@
       </c>
       <c r="I5" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="S5" s="9" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Add prize and prize detail test case
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PathmazingPC\Stars\appiumtest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D849205A-6436-4E74-967D-D922F771EEA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7F1868-3F5C-4AA3-87B1-805EBAC3744F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="1800" windowWidth="27675" windowHeight="12840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="userData" sheetId="1" r:id="rId1"/>
+    <sheet name="orgData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
   <si>
     <t>User Name</t>
   </si>
@@ -130,13 +131,52 @@
   </si>
   <si>
     <t xml:space="preserve">I have to go to the bank tomorrow </t>
+  </si>
+  <si>
+    <t>Organization Data</t>
+  </si>
+  <si>
+    <t>Prize</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Coke Can 330ml</t>
+  </si>
+  <si>
+    <t>In-stock</t>
+  </si>
+  <si>
+    <t>Coca-Cola, or Coke, is a carbonated soft drink manufactured by The Coca-Cola Company</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>One Plus 8 Pro</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Operating System: OxygenOS based on Android™ 10. CPU: Qualcomm® Snapdragon™ 865. 5G</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,8 +223,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -194,6 +242,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -211,7 +265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -219,13 +273,17 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -509,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S9" sqref="S9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,17 +593,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B2"/>
@@ -586,58 +656,58 @@
       <c r="AE3" s="4"/>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="11" t="s">
+      <c r="L4" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="M4" s="11" t="s">
+      <c r="M4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="11" t="s">
+      <c r="N4" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="O4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="11" t="s">
+      <c r="P4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="Q4" s="11" t="s">
+      <c r="Q4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="R4" s="11" t="s">
+      <c r="R4" s="10" t="s">
         <v>24</v>
       </c>
       <c r="S4" s="6" t="s">
@@ -676,13 +746,13 @@
       <c r="J5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="L5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M5" s="8" t="s">
+      <c r="M5" s="7" t="s">
         <v>27</v>
       </c>
       <c r="N5" s="1" t="s">
@@ -695,16 +765,16 @@
       <c r="Q5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="R5" s="9" t="s">
+      <c r="R5" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="9" t="s">
+      <c r="S5" s="8" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A1:U1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" xr:uid="{E33C78A5-8AFA-40DF-ABB6-00060D58097A}"/>
@@ -713,4 +783,556 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1D2823-CB1F-4CEA-8F2D-744EBB05B100}">
+  <dimension ref="A1:X21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:W1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
-Add Staff List Testcase and update Prizes Details
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PathmazingPC\Stars\appiumtest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PathmazingPC\Stars\Stars-Automation-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7F1868-3F5C-4AA3-87B1-805EBAC3744F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26356BE9-3F21-4600-A52A-80AA8D729F52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="1800" windowWidth="27675" windowHeight="12840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1035" yWindow="2490" windowWidth="27675" windowHeight="12840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="userData" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>User Name</t>
   </si>
@@ -170,6 +170,36 @@
   </si>
   <si>
     <t>Operating System: OxygenOS based on Android™ 10. CPU: Qualcomm® Snapdragon™ 865. 5G</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Total Staff</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>Staff List</t>
+  </si>
+  <si>
+    <t>Alvin Meta</t>
+  </si>
+  <si>
+    <t>Android Developer</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Oliver Sovann</t>
+  </si>
+  <si>
+    <t>Project Manager Assistant</t>
   </si>
 </sst>
 </file>
@@ -265,7 +295,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -278,6 +308,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -565,246 +596,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AE5"/>
+  <dimension ref="B1:AF40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" style="1" customWidth="1"/>
-    <col min="10" max="11" width="11.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.5703125" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13" customWidth="1"/>
-    <col min="16" max="16" width="11.5703125" customWidth="1"/>
-    <col min="17" max="17" width="11.7109375" customWidth="1"/>
-    <col min="18" max="18" width="23.140625" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19" style="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" customWidth="1"/>
+    <col min="11" max="12" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="17" max="17" width="11.5703125" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="23.140625" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="2:32" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-    </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="B2"/>
-    </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4"/>
-    </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="L4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="M4" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="R4" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="T4" s="6"/>
-    </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:U1"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{E33C78A5-8AFA-40DF-ABB6-00060D58097A}"/>
-    <hyperlink ref="D5" r:id="rId2" xr:uid="{9203AC28-A818-4032-B9E9-1FE079B72FCE}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1D2823-CB1F-4CEA-8F2D-744EBB05B100}">
-  <dimension ref="A1:X21"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="13"/>
       <c r="C1" s="13"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
@@ -825,7 +648,261 @@
       <c r="T1" s="13"/>
       <c r="U1" s="13"/>
       <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
+    </row>
+    <row r="2" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+      <c r="U2" s="4"/>
+      <c r="V2" s="4"/>
+      <c r="W2" s="4"/>
+      <c r="X2" s="4"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="4"/>
+      <c r="AA2" s="4"/>
+      <c r="AB2" s="4"/>
+      <c r="AC2" s="4"/>
+      <c r="AD2" s="4"/>
+      <c r="AE2" s="4"/>
+      <c r="AF2" s="4"/>
+    </row>
+    <row r="3" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="R3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="6"/>
+    </row>
+    <row r="4" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="T4" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:V1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{E33C78A5-8AFA-40DF-ABB6-00060D58097A}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{9203AC28-A818-4032-B9E9-1FE079B72FCE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1D2823-CB1F-4CEA-8F2D-744EBB05B100}">
+  <dimension ref="A1:X21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -991,7 +1068,9 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>49</v>
+      </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
@@ -1017,8 +1096,12 @@
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>51</v>
+      </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -1069,7 +1152,9 @@
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -1095,9 +1180,15 @@
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
@@ -1121,9 +1212,15 @@
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -1147,9 +1244,15 @@
       <c r="X14" s="1"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>

</xml_diff>

<commit_message>
-Complete Staff List Test Case
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PathmazingPC\Stars\Stars-Automation-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26356BE9-3F21-4600-A52A-80AA8D729F52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CA0BD2-38B2-4FE0-92B1-A08C9BE56AD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1035" yWindow="2490" windowWidth="27675" windowHeight="12840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="435" yWindow="1995" windowWidth="27675" windowHeight="12840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="userData" sheetId="1" r:id="rId1"/>
     <sheet name="orgData" sheetId="2" r:id="rId2"/>
+    <sheet name="staffList" sheetId="3" r:id="rId3"/>
+    <sheet name="teamList" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="92">
   <si>
     <t>User Name</t>
   </si>
@@ -200,6 +202,108 @@
   </si>
   <si>
     <t>Project Manager Assistant</t>
+  </si>
+  <si>
+    <t>Ella</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Alvin</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Pheak</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Thavy</t>
+  </si>
+  <si>
+    <t>Chief Executive Officer</t>
+  </si>
+  <si>
+    <t>Chief Operation Officer</t>
+  </si>
+  <si>
+    <t>Chief Technology Officer</t>
+  </si>
+  <si>
+    <t>Chief Financial Officer</t>
+  </si>
+  <si>
+    <t>Lead QA Tester</t>
+  </si>
+  <si>
+    <t>Accountant</t>
+  </si>
+  <si>
+    <t>Lead Android Developer</t>
+  </si>
+  <si>
+    <t>Photoshop Manager</t>
+  </si>
+  <si>
+    <t>Photo Editor</t>
+  </si>
+  <si>
+    <t>Wesley</t>
+  </si>
+  <si>
+    <t>iOS Lead</t>
+  </si>
+  <si>
+    <t>Roy</t>
+  </si>
+  <si>
+    <t>iOS Developer</t>
+  </si>
+  <si>
+    <t>Steven Path</t>
+  </si>
+  <si>
+    <t>Logan Sean</t>
+  </si>
+  <si>
+    <t>Nick Nuth</t>
+  </si>
+  <si>
+    <t>Rachel Chan</t>
+  </si>
+  <si>
+    <t>Ethan Cheat</t>
+  </si>
+  <si>
+    <t>Total Team</t>
+  </si>
+  <si>
+    <t>Stars Team</t>
+  </si>
+  <si>
+    <t>Coke Team</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>5 Members</t>
+  </si>
+  <si>
+    <t>Ryan Soy</t>
+  </si>
+  <si>
+    <t>Wesley Lim</t>
+  </si>
+  <si>
+    <t>Total Member</t>
+  </si>
+  <si>
+    <t>Stars</t>
   </si>
 </sst>
 </file>
@@ -295,7 +399,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -309,12 +413,25 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -598,7 +715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AF40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -625,29 +742,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
     </row>
     <row r="2" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -866,8 +983,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1D2823-CB1F-4CEA-8F2D-744EBB05B100}">
   <dimension ref="A1:X21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,31 +995,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1438,4 +1555,407 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B323882-22C3-4EE6-9699-EF3DECCADCAE}">
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.42578125" style="13" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="13">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="13">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="13">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="13">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="13">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="13">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="13">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D4FDEE-3088-47E6-84EE-65825F492215}">
+  <dimension ref="A1:M21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12" style="1" customWidth="1"/>
+    <col min="5" max="13" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="18"/>
+      <c r="D4" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="D5" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="18"/>
+      <c r="E6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="18"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="18"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="18"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="18"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="18"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="18"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="18"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
-Configure Testcase XML file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PathmazingPC\Stars\Stars-Automation-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04CA0BD2-38B2-4FE0-92B1-A08C9BE56AD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56A0788-793D-4165-AC12-69FBE32B404E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="435" yWindow="1995" windowWidth="27675" windowHeight="12840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="1590" windowWidth="27675" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="userData" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="93">
   <si>
     <t>User Name</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Operating System: OxygenOS based on Android™ 10. CPU: Qualcomm® Snapdragon™ 865. 5G</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Staff</t>
   </si>
   <si>
@@ -304,6 +301,12 @@
   </si>
   <si>
     <t>Stars</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>9</t>
   </si>
 </sst>
 </file>
@@ -416,6 +419,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -428,10 +435,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -715,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AF40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -742,29 +745,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
     </row>
     <row r="2" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -882,8 +885,8 @@
       </c>
     </row>
     <row r="16" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>48</v>
+      <c r="B16" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
@@ -903,7 +906,7 @@
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
@@ -923,7 +926,7 @@
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
@@ -995,31 +998,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1186,7 +1189,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1214,10 +1217,10 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1270,7 +1273,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1298,13 +1301,13 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1333,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>25</v>
@@ -1362,13 +1365,13 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1574,20 +1577,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="A1" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1595,10 +1598,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1609,10 +1612,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1623,10 +1626,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1637,10 +1640,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1651,10 +1654,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
         <v>56</v>
-      </c>
-      <c r="C7" t="s">
-        <v>57</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1665,10 +1668,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1679,10 +1682,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1693,10 +1696,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
         <v>74</v>
-      </c>
-      <c r="C10" t="s">
-        <v>75</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1707,10 +1710,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1735,10 +1738,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C13" t="s">
         <v>76</v>
-      </c>
-      <c r="C13" t="s">
-        <v>77</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1749,10 +1752,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1763,10 +1766,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1777,10 +1780,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1791,10 +1794,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1805,10 +1808,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1827,7 +1830,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D4FDEE-3088-47E6-84EE-65825F492215}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
@@ -1840,116 +1843,116 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="A1" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="C3" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="18">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
+      <c r="A4" s="14"/>
       <c r="D4" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="14"/>
+      <c r="D5" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="D5" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
+      <c r="A6" s="14"/>
       <c r="E6" s="12">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="18">
+      <c r="A7" s="14">
         <v>2</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
+      <c r="A8" s="14"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
+      <c r="A9" s="14"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="18"/>
+      <c r="A10" s="14"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
+      <c r="A11" s="14"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
+      <c r="A12" s="14"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="18"/>
+      <c r="A13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="18"/>
+      <c r="A14" s="14"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
+      <c r="A15" s="14"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="18"/>
+      <c r="A16" s="14"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18"/>
+      <c r="A17" s="14"/>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18"/>
+      <c r="A18" s="14"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18"/>
+      <c r="A19" s="14"/>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18"/>
+      <c r="A20" s="14"/>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18"/>
+      <c r="A21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
-Update Profile test cases
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PathmazingPC\Stars\Stars-Automation-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56A0788-793D-4165-AC12-69FBE32B404E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6E2125-2CEC-4F7E-9F0B-7265F86B6B40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="1590" windowWidth="27675" windowHeight="12840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="userData" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="103">
   <si>
     <t>User Name</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Last Month</t>
   </si>
   <si>
-    <t>All Time</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
@@ -66,9 +63,6 @@
     <t>Phone number</t>
   </si>
   <si>
-    <t>099100103</t>
-  </si>
-  <si>
     <t>USER Data</t>
   </si>
   <si>
@@ -276,37 +270,73 @@
     <t>Ethan Cheat</t>
   </si>
   <si>
-    <t>Total Team</t>
-  </si>
-  <si>
     <t>Stars Team</t>
   </si>
   <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Ryan Soy</t>
+  </si>
+  <si>
+    <t>Wesley Lim</t>
+  </si>
+  <si>
+    <t>Total Member</t>
+  </si>
+  <si>
+    <t>Stars</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>Repairancy Team</t>
+  </si>
+  <si>
+    <t>3 Members</t>
+  </si>
+  <si>
+    <t>2 Members</t>
+  </si>
+  <si>
+    <t>1 Member</t>
+  </si>
+  <si>
+    <t>Alvin Sreng</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
     <t>Coke Team</t>
   </si>
   <si>
-    <t>Member</t>
-  </si>
-  <si>
-    <t>5 Members</t>
-  </si>
-  <si>
-    <t>Ryan Soy</t>
-  </si>
-  <si>
-    <t>Wesley Lim</t>
-  </si>
-  <si>
-    <t>Total Member</t>
-  </si>
-  <si>
-    <t>Stars</t>
-  </si>
-  <si>
-    <t>45</t>
-  </si>
-  <si>
-    <t>9</t>
+    <t>Earned All Time</t>
+  </si>
+  <si>
+    <t>User ID</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>+85599100103</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>07/07/2019</t>
+  </si>
+  <si>
+    <t>1 year, 14 days</t>
+  </si>
+  <si>
+    <t>Phnompenh</t>
   </si>
 </sst>
 </file>
@@ -402,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -422,7 +452,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,6 +465,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -716,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AF40"/>
+  <dimension ref="B1:AF52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +777,7 @@
   <sheetData>
     <row r="1" spans="2:32" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
@@ -771,7 +802,7 @@
     </row>
     <row r="2" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -809,22 +840,22 @@
         <v>0</v>
       </c>
       <c r="O3" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="10" t="s">
+      <c r="R3" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="Q3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="R3" s="10" t="s">
+      <c r="S3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="S3" s="10" t="s">
-        <v>24</v>
-      </c>
       <c r="T3" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="U3" s="6"/>
     </row>
@@ -833,20 +864,20 @@
         <v>1</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>31</v>
-      </c>
       <c r="T4" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="2:32" x14ac:dyDescent="0.25">
@@ -856,17 +887,17 @@
     </row>
     <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B9" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="2:32" x14ac:dyDescent="0.25">
@@ -886,7 +917,7 @@
     </row>
     <row r="16" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
@@ -896,17 +927,17 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
@@ -916,57 +947,103 @@
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" s="9" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B34" s="7" t="s">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="12" t="s">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="20"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C46" s="20"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+    </row>
+    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="7" t="s">
-        <v>27</v>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -999,7 +1076,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
@@ -1026,7 +1103,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="11"/>
@@ -1035,16 +1112,16 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1069,16 +1146,16 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>42</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1103,16 +1180,16 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1189,7 +1266,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1217,10 +1294,10 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1273,7 +1350,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1301,13 +1378,13 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1336,10 +1413,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1365,13 +1442,13 @@
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1578,7 +1655,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -1590,7 +1667,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1598,10 +1675,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1612,10 +1689,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1626,10 +1703,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1640,10 +1717,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1654,10 +1731,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1668,10 +1745,10 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -1682,10 +1759,10 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -1696,10 +1773,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -1710,10 +1787,10 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -1727,7 +1804,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D12">
         <v>40</v>
@@ -1738,10 +1815,10 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -1752,10 +1829,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -1766,10 +1843,10 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -1780,10 +1857,10 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -1794,10 +1871,10 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -1808,10 +1885,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -1828,23 +1905,24 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D4FDEE-3088-47E6-84EE-65825F492215}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="3" width="14.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="1" customWidth="1"/>
     <col min="5" max="13" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
@@ -1855,18 +1933,20 @@
       <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="14"/>
+      <c r="A2" s="14" t="s">
+        <v>93</v>
+      </c>
       <c r="B2" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="D2" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="15" t="s">
         <v>85</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1874,10 +1954,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>1</v>
@@ -1886,31 +1966,20 @@
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14"/>
       <c r="D4" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14"/>
       <c r="D5" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="14"/>
-      <c r="E6" s="12">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="14">
-        <v>2</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>86</v>
-      </c>
+      <c r="A7" s="14"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
@@ -1926,12 +1995,29 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
+      <c r="E12" s="12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="14">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="14"/>
+      <c r="D14" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
@@ -1939,20 +2025,76 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="14"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="14"/>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="14"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="14"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="14"/>
+      <c r="E22" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="14"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="14"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="14"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="14"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="14"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="14"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="14"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="14"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="14"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="14"/>
+      <c r="E33" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
-Update Reward Staff Test Case
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PathmazingPC\Stars\Stars-Automation-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6E2125-2CEC-4F7E-9F0B-7265F86B6B40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151F6104-CC5B-43D1-8CC5-DE93399B49E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="userData" sheetId="1" r:id="rId1"/>
     <sheet name="orgData" sheetId="2" r:id="rId2"/>
     <sheet name="staffList" sheetId="3" r:id="rId3"/>
     <sheet name="teamList" sheetId="4" r:id="rId4"/>
+    <sheet name="rewardStaff" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="124">
   <si>
     <t>User Name</t>
   </si>
@@ -337,6 +338,69 @@
   </si>
   <si>
     <t>Phnompenh</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Reward List</t>
+  </si>
+  <si>
+    <t>Reward Categories</t>
+  </si>
+  <si>
+    <t>Very Good</t>
+  </si>
+  <si>
+    <t>Stars to Reward</t>
+  </si>
+  <si>
+    <t>Reward Reason</t>
+  </si>
+  <si>
+    <t>Receiver List</t>
+  </si>
+  <si>
+    <t>Categories Name</t>
+  </si>
+  <si>
+    <t>Effort: Extraordinary</t>
+  </si>
+  <si>
+    <t>Effort: Very Good</t>
+  </si>
+  <si>
+    <t>Effort: Good</t>
+  </si>
+  <si>
+    <t>Question: Extraordinary</t>
+  </si>
+  <si>
+    <t>Question: Very Good</t>
+  </si>
+  <si>
+    <t>Question: Good</t>
+  </si>
+  <si>
+    <t>Idea: Extraordinary</t>
+  </si>
+  <si>
+    <t>Idea: Very Good</t>
+  </si>
+  <si>
+    <t>Idea: Good</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you for your commitment on update the stars new feature. Reward Case: </t>
   </si>
 </sst>
 </file>
@@ -432,7 +496,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -453,6 +517,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -465,7 +530,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -749,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:AF52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,29 +844,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="16"/>
-      <c r="M1" s="16"/>
-      <c r="N1" s="16"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
-      <c r="T1" s="16"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="16"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
     </row>
     <row r="2" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -927,7 +995,7 @@
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>8</v>
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
@@ -1014,17 +1082,17 @@
       <c r="B45" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C45" s="20"/>
+      <c r="C45" s="16"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="20"/>
+      <c r="C46" s="16"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
@@ -1075,31 +1143,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -1642,7 +1710,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD18"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1654,16 +1722,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -1907,7 +1975,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D4FDEE-3088-47E6-84EE-65825F492215}">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -1921,16 +1989,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -2103,4 +2171,165 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C38E45E-BA72-4F84-9972-2894A4F71DDE}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="73.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="22"/>
+    <col min="7" max="7" width="31" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="G5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D8" s="10"/>
+      <c r="G8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
-Update Reward Peer Test Case
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -3,25 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PathmazingPC\Stars\Stars-Automation-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC13F9D-38E0-4E3A-AEAD-023B01237501}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF81685-C41A-4749-A901-CE9AF93C2A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10785" yWindow="2595" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="userData" sheetId="1" r:id="rId1"/>
-    <sheet name="orgData" sheetId="2" r:id="rId2"/>
-    <sheet name="staffList" sheetId="3" r:id="rId3"/>
-    <sheet name="teamList" sheetId="4" r:id="rId4"/>
-    <sheet name="rewardStaff" sheetId="5" r:id="rId5"/>
+    <sheet name="userManager" sheetId="8" r:id="rId2"/>
+    <sheet name="rewardCat" sheetId="6" r:id="rId3"/>
+    <sheet name="orgData" sheetId="2" r:id="rId4"/>
+    <sheet name="staffList" sheetId="3" r:id="rId5"/>
+    <sheet name="teamList" sheetId="4" r:id="rId6"/>
+    <sheet name="rewardStaff" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="134">
   <si>
     <t>User Name</t>
   </si>
@@ -385,41 +387,58 @@
     <t>Idea: Extraordinary</t>
   </si>
   <si>
+    <t>Idea: Good</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thank you for your commitment on update the stars new feature. Reward Case: </t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>9:30 PM</t>
+  </si>
+  <si>
+    <t>Approve Time</t>
+  </si>
+  <si>
+    <t>Request Time</t>
+  </si>
+  <si>
     <t>Idea: Very Good</t>
   </si>
   <si>
-    <t>Idea: Good</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t>25</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thank you for your commitment on update the stars new feature. Reward Case: </t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>130</t>
+    <t>3:26 PM</t>
+  </si>
+  <si>
+    <t>Oliver.pa@mailinator.com</t>
+  </si>
+  <si>
+    <t>Sovann monynith</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>+85599100105</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -509,7 +528,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -547,6 +566,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -828,32 +848,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:AF52"/>
+  <dimension ref="A1:AF52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B52" sqref="B2:B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="42.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="24.85546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="12.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="1" width="18.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="16.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="11" max="12" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="12.7109375" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="1" max="1" width="4.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="42.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="16.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="13" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="17.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1006,14 +1026,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
@@ -1087,7 +1107,7 @@
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="12" t="s">
         <v>96</v>
       </c>
     </row>
@@ -1097,7 +1117,7 @@
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="12" t="s">
         <v>99</v>
       </c>
       <c r="C45" s="16"/>
@@ -1113,7 +1133,7 @@
       <c r="D47" s="16"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="23" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1123,7 +1143,7 @@
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="12" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1146,18 +1166,398 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30579CF5-48B0-4FB8-BA89-654746A3E700}">
+  <dimension ref="A1:N52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B15" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" s="1"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" s="9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" s="1"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="1"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" s="23" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="1"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:N1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B7" r:id="rId1" xr:uid="{0133F880-22BA-4DCE-BA92-709D6DE6E972}"/>
+    <hyperlink ref="B13" r:id="rId2" xr:uid="{D8F26AE1-F1CF-46E7-BBBB-991572B99390}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29CCC670-BA82-4E92-9506-8AB2516D93C7}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D1D2823-CB1F-4CEA-8F2D-744EBB05B100}">
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1723,7 +2123,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B323882-22C3-4EE6-9699-EF3DECCADCAE}">
   <dimension ref="A1:H18"/>
   <sheetViews>
@@ -1733,10 +2133,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="13" width="4.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="27.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="1" max="1" width="4.42578125" style="13" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.5703125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1989,9 +2389,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65D4FDEE-3088-47E6-84EE-65825F492215}">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
@@ -1999,11 +2399,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="1" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="5" max="13" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="1" collapsed="1"/>
+    <col min="2" max="2" width="19.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="13" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -2191,21 +2591,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C38E45E-BA72-4F84-9972-2894A4F71DDE}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="73.140625" collapsed="true"/>
-    <col min="5" max="5" style="17" width="9.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="31.0" collapsed="true"/>
-    <col min="8" max="8" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="73.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.140625" style="17" collapsed="1"/>
+    <col min="7" max="7" width="31" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -2216,9 +2616,7 @@
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
       <c r="E1" s="22"/>
-      <c r="F1" s="22" t="s">
-        <v>105</v>
-      </c>
+      <c r="F1" s="22"/>
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
       <c r="I1" s="22"/>
@@ -2228,103 +2626,44 @@
       <c r="A3" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="F3" t="s">
-        <v>110</v>
-      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G5" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>5</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" s="10"/>
-      <c r="G8" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>120</v>
+      <c r="B11" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -2340,6 +2679,26 @@
       </c>
       <c r="C14" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Update Reward Superior Test Case
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PathmazingPC\Stars\Stars-Automation-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF81685-C41A-4749-A901-CE9AF93C2A1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE7125C-564C-47CB-AF33-6994CE344DB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10785" yWindow="2595" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="userData" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="136">
   <si>
     <t>User Name</t>
   </si>
@@ -402,44 +402,50 @@
     <t xml:space="preserve">Thank you for your commitment on update the stars new feature. Reward Case: </t>
   </si>
   <si>
+    <t>9:30 PM</t>
+  </si>
+  <si>
+    <t>Approve Time</t>
+  </si>
+  <si>
+    <t>Request Time</t>
+  </si>
+  <si>
+    <t>Idea: Very Good</t>
+  </si>
+  <si>
+    <t>Oliver.pa@mailinator.com</t>
+  </si>
+  <si>
+    <t>Sovann monynith</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>+85599100105</t>
+  </si>
+  <si>
+    <t>500</t>
+  </si>
+  <si>
+    <t>11:31 AM</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
     <t>200</t>
-  </si>
-  <si>
-    <t>9:30 PM</t>
-  </si>
-  <si>
-    <t>Approve Time</t>
-  </si>
-  <si>
-    <t>Request Time</t>
-  </si>
-  <si>
-    <t>Idea: Very Good</t>
-  </si>
-  <si>
-    <t>3:26 PM</t>
-  </si>
-  <si>
-    <t>Oliver.pa@mailinator.com</t>
-  </si>
-  <si>
-    <t>Sovann monynith</t>
-  </si>
-  <si>
-    <t>Project Manager</t>
-  </si>
-  <si>
-    <t>0002</t>
-  </si>
-  <si>
-    <t>+85599100105</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,6 +496,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -551,8 +563,12 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -563,10 +579,6 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -850,8 +862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B52" sqref="B2:B52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,29 +889,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
     </row>
     <row r="2" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -1027,13 +1039,13 @@
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>119</v>
+      <c r="B19" s="1" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
@@ -1133,7 +1145,7 @@
       <c r="D47" s="16"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="23" t="s">
+      <c r="B48" s="18" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1156,6 +1168,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:V1"/>
   </mergeCells>
+  <phoneticPr fontId="7" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B7" r:id="rId1" xr:uid="{E33C78A5-8AFA-40DF-ABB6-00060D58097A}"/>
     <hyperlink ref="B13" r:id="rId2" xr:uid="{9203AC28-A818-4032-B9E9-1FE079B72FCE}"/>
@@ -1169,31 +1182,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30579CF5-48B0-4FB8-BA89-654746A3E700}">
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
@@ -1220,7 +1233,7 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1233,7 +1246,7 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1326,7 +1339,7 @@
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
@@ -1339,7 +1352,7 @@
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
@@ -1378,7 +1391,7 @@
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
@@ -1398,7 +1411,7 @@
       <c r="B47" s="1"/>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B48" s="23" t="s">
+      <c r="B48" s="18" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1437,7 +1450,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,13 +1459,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="1"/>
@@ -1523,7 +1536,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>119</v>
@@ -1561,31 +1574,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="21"/>
+      <c r="U1" s="21"/>
+      <c r="V1" s="21"/>
+      <c r="W1" s="21"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
@@ -2140,16 +2153,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
@@ -2407,16 +2420,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
@@ -2609,18 +2622,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -2657,7 +2670,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>41</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2683,22 +2696,22 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
-Update Reward Subordinate Test Case
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PathmazingPC\Stars\Stars-Automation-Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE7125C-564C-47CB-AF33-6994CE344DB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BFEB90-D0BA-4BAA-BC9B-9C80E04D5BC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="134">
   <si>
     <t>User Name</t>
   </si>
@@ -429,16 +429,10 @@
     <t>+85599100105</t>
   </si>
   <si>
-    <t>500</t>
-  </si>
-  <si>
     <t>11:31 AM</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>200</t>
+    <t>900</t>
   </si>
 </sst>
 </file>
@@ -863,7 +857,7 @@
   <dimension ref="A1:AF52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,14 +1032,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
-        <v>135</v>
+    <row r="19" spans="2:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>180</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
@@ -2670,7 +2664,7 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>134</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2711,7 +2705,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>